<commit_message>
Replaced hurtsMe flag with HurtOnInteract Interaction
</commit_message>
<xml_diff>
--- a/Unnamed Platformer Plan.xlsx
+++ b/Unnamed Platformer Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22980" windowHeight="10875" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="23265" windowHeight="7845"/>
   </bookViews>
   <sheets>
     <sheet name="Todo" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$23</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:X34"/>
+  <oleSize ref="A1:L23"/>
 </workbook>
 </file>
 
@@ -189,12 +189,6 @@
     <t>Brainstorm and implement win feedback</t>
   </si>
   <si>
-    <t>Brainstorm and list methods of procedurally generating areas (then prototype the best ones first according to criteria)</t>
-  </si>
-  <si>
-    <t>Brainstorm and list item types for the game; add to do todo the most interesting ashighest priority</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
@@ -283,6 +277,12 @@
   </si>
   <si>
     <t>Other types:</t>
+  </si>
+  <si>
+    <t>Brainstorm and list item types for the game; add the most interesting as highest priority todos</t>
+  </si>
+  <si>
+    <t>Improve variety of procedurally generated levels</t>
   </si>
 </sst>
 </file>
@@ -674,9 +674,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,13 +700,13 @@
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -761,7 +761,7 @@
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -984,10 +984,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>20</v>
@@ -998,15 +998,15 @@
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CP25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BD11" sqref="BD11"/>
     </sheetView>
   </sheetViews>
@@ -1219,449 +1219,449 @@
   <sheetData>
     <row r="1" spans="1:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK1" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BG2" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="BK2" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK3" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="BX3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BY3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BZ3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CA3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CB3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CC3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CD3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CE3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK4" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="BW4" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BV5" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="BV5" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U6" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="BK6" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="BU6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BT7" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="BT7" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="BZ7" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BJ8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BK8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BL8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BM8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BN8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BO8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BP8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BQ8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BR8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BS8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BT8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BU8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BV8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BW8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BX8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BY8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BZ8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CA8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CB8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CC8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CD8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CE8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CF8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="CG8" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ9" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="BJ9" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="T10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q10" s="6" t="s">
+      <c r="AO10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="BJ10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="T10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AO10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="BJ10" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="BZ10" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="U11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="U11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="BJ11" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="BN11" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="U12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="U12" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="AH12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AI12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AJ12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AR12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AS12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AT12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AU12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AV12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AW12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AX12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AY12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AZ12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BA12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BB12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BC12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BD12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BE12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BF12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BG12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BH12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BI12" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BJ12" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U13" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AG13" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AM13" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AW13" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J14" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AF14" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AX14" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U15" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="X15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="W15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="X15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AY15" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="BW15" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AZ16" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="BA16" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BB16" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BC16" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BD16" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BE16" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BF16" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BG16" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BY16" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CA17" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AP18" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="CA18" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CB19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="CI19" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="CI19" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="20" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="Q20" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="CB20" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q21" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added dev hotkey F3 to generate a random game
</commit_message>
<xml_diff>
--- a/Unnamed Platformer Plan.xlsx
+++ b/Unnamed Platformer Plan.xlsx
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Brainstorming!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$23</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <oleSize ref="A1:L33"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="108">
   <si>
     <t>1. Implement level serialization</t>
   </si>
@@ -155,9 +155,6 @@
   </si>
   <si>
     <t>Implement choosing the shape of the collision polygon (circle/square)</t>
-  </si>
-  <si>
-    <t>Implement generation of polygons from image masks (1 - create polygon from coordinates of edge pixels; 2 - remove points from polygon and see how much area is reduced; 3 - if area is reduced &lt; x%, allow point removal</t>
   </si>
   <si>
     <t>Slope Physics</t>
@@ -358,6 +355,12 @@
   </si>
   <si>
     <t>Performance</t>
+  </si>
+  <si>
+    <t>Rework object hierarchy to require less work on changing textures or types</t>
+  </si>
+  <si>
+    <t>Implement image mask -&gt; polygon (1 - create polygon from coordinates of edge pixels; 2 - remove points from polygon and see how much area is reduced; 3 - if area is reduced &lt; x%, allow point removal</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -438,6 +441,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,17 +756,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="111.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -773,465 +782,488 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>31</v>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
+      <c r="B6" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>87</v>
+      <c r="B7" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>87</v>
+      <c r="B9" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>3</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>87</v>
+      <c r="B10" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>87</v>
+      <c r="B11" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>87</v>
+      <c r="B12" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>87</v>
+      <c r="B13" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>87</v>
+      <c r="B14" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>87</v>
+      <c r="B15" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>3</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>87</v>
+      <c r="B16" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>2</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>24</v>
+      <c r="C18" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>2</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>29</v>
+      <c r="B19" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>2</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>35</v>
+      <c r="B20" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>2</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>39</v>
+      <c r="C21" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>2</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>38</v>
+      <c r="C22" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>2</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>34</v>
+      <c r="B23" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>2</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>45</v>
+      <c r="B25" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>2</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>2</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>85</v>
+      <c r="C26" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>87</v>
+      <c r="B27" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>2</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>87</v>
+      <c r="B28" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>2</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>87</v>
+      <c r="B29" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>2</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>87</v>
+      <c r="B30" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>2</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>87</v>
+      <c r="B31" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>2</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>87</v>
+      <c r="B32" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>2</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>87</v>
+      <c r="B33" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>1</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>25</v>
+      <c r="A34" s="2">
+        <v>2</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>1</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>1</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>29</v>
+      <c r="B36" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>1</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>50</v>
+      <c r="B37" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>1</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>41</v>
+      <c r="B38" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>0</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>0</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>34</v>
+      <c r="B40" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>0</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>0</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+    <row r="43" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>0</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="B43" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="9"/>
+    </row>
+    <row r="45" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="9"/>
+    </row>
+    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="9"/>
+    </row>
+    <row r="48" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="9"/>
+    </row>
+    <row r="49" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="9"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C22">
+  <autoFilter ref="A1:C23">
     <sortState ref="A2:C43">
       <sortCondition descending="1" ref="A1:A23"/>
     </sortState>
@@ -1273,10 +1305,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>20</v>
@@ -1287,18 +1319,18 @@
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1405,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1511,449 +1543,449 @@
   <sheetData>
     <row r="1" spans="1:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK1" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BG2" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BK2" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BX3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BY3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BZ3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CA3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CB3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CC3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CD3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CE3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BW4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK5" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BV5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U6" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BK6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BU6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK7" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BT7" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="BZ7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BJ8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BK8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BL8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BM8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BN8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BO8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BP8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BQ8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BR8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BS8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BT8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BU8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BV8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BW8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BX8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BY8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BZ8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CA8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CB8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CC8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CD8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CE8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CF8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="CG8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="BJ9" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="BJ9" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q10" s="6" t="s">
+      <c r="T10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="AO10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="BJ10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AO10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="BJ10" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="BZ10" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="U11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="U11" s="6" t="s">
+      <c r="BJ11" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="BJ11" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="BN11" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="U12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AS12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AX12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AY12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BB12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BC12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BD12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BF12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BH12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BJ12" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AW12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BB12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BC12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BD12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BE12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BF12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BG12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BH12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BI12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BJ12" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AG13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AW13" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="AM13" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW13" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J14" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX14" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="AX14" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U15" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="X15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="W15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="X15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE15" s="6" t="s">
+      <c r="AY15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AY15" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="BW15" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AZ16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BA16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BB16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BC16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BD16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BE16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BF16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BG16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BY16" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CA17" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AP18" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="CA18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CB19" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="CI19" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="Q20" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="CB20" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q21" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Replaced several hashmaps with enummaps; miscellaneous tweaking
</commit_message>
<xml_diff>
--- a/Unnamed Platformer Plan.xlsx
+++ b/Unnamed Platformer Plan.xlsx
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Brainstorming!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$20</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <oleSize ref="A1:L33"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="103">
   <si>
     <t>1. Implement level serialization</t>
   </si>
@@ -119,12 +119,6 @@
   </si>
   <si>
     <t>Improve spring physics</t>
-  </si>
-  <si>
-    <t>Improve jumping physics</t>
-  </si>
-  <si>
-    <t>Implement direction-based interactions for spikes and etc.</t>
   </si>
   <si>
     <t>Physics</t>
@@ -198,9 +192,6 @@
     <t>Game mechanic</t>
   </si>
   <si>
-    <t>Procedural Generation</t>
-  </si>
-  <si>
     <t>[</t>
   </si>
   <si>
@@ -277,18 +268,6 @@
   </si>
   <si>
     <t>Improve variety of procedurally generated levels</t>
-  </si>
-  <si>
-    <t>Data mine classic platformer levels for section patterns correlated to:
-- Previous sections
-- Difficulty level
-- Established level gimmicks
-Also take note of new types of sections
-Also take note of how to represent each type of section in a data structure (maybe use an array of objects mapped to points relating to the grid?)
-Also take note of how item placement may or may not be dependent on section type</t>
-  </si>
-  <si>
-    <t>strict vs loose side interaction</t>
   </si>
   <si>
     <t>object tile chains/grids</t>
@@ -760,7 +739,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,43 +766,43 @@
         <v>4</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="2">
         <v>3</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>31</v>
+      <c r="B3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>32</v>
+      <c r="B4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>33</v>
+      <c r="B5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -831,10 +810,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -842,10 +821,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -853,10 +832,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -864,10 +843,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -875,10 +854,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -886,10 +865,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -897,10 +876,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -908,65 +887,65 @@
         <v>3</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="5">
         <v>3</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>93</v>
+      <c r="B14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="5">
         <v>3</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>94</v>
+      <c r="B15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>3</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>96</v>
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="5">
         <v>2</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>81</v>
+      <c r="B18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -974,10 +953,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -985,76 +964,76 @@
         <v>2</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="2">
         <v>2</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>50</v>
+      <c r="B21" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="2">
         <v>2</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>39</v>
+      <c r="B22" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="2">
         <v>2</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>38</v>
+      <c r="B23" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="2">
         <v>2</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>42</v>
+      <c r="B24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="2">
         <v>2</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="B25" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>2</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>107</v>
+      <c r="B26" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1062,10 +1041,10 @@
         <v>2</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1073,76 +1052,76 @@
         <v>2</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="5">
         <v>2</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="B29" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
         <v>2</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>99</v>
+      <c r="B30" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="5">
         <v>2</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>100</v>
+      <c r="B31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>2</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>101</v>
+      <c r="A32" s="5">
+        <v>1</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>2</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>102</v>
+      <c r="A33" s="5">
+        <v>1</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>2</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>103</v>
+      <c r="A34" s="5">
+        <v>1</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1153,7 +1132,7 @@
         <v>27</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1161,43 +1140,43 @@
         <v>1</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
-        <v>1</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>48</v>
+      <c r="A38" s="2">
+        <v>0</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1205,44 +1184,20 @@
         <v>0</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>0</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>0</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="B42" s="9"/>
     </row>
     <row r="43" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>0</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="B43" s="9"/>
     </row>
     <row r="44" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
@@ -1263,9 +1218,9 @@
       <c r="B49" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C23">
-    <sortState ref="A2:C43">
-      <sortCondition descending="1" ref="A1:A23"/>
+  <autoFilter ref="A1:C20">
+    <sortState ref="A2:C40">
+      <sortCondition descending="1" ref="A1:A20"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:A1048576">
@@ -1291,7 +1246,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,10 +1260,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>20</v>
@@ -1317,22 +1272,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="C3" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1353,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1543,449 +1491,449 @@
   <sheetData>
     <row r="1" spans="1:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK1" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BG2" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="BK2" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK3" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="BX3" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BY3" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BZ3" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CA3" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CB3" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CC3" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CD3" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CE3" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK4" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="BW4" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK5" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="BV5" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U6" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="BK6" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="BU6" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK7" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="BT7" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="BZ7" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BJ8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BK8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BL8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BM8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BN8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BO8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BP8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BQ8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BR8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BS8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BT8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BU8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BV8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BW8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BX8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BY8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BZ8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CA8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CB8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CC8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CD8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CE8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CF8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="CG8" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R9" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="BJ9" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="T10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BJ10" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="BZ10" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J11" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="U11" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="BJ11" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="BN11" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="U12" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="AH12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AI12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AJ12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AR12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AS12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AT12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AU12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AV12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AW12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AX12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AY12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AZ12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BA12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BB12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BC12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BD12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BE12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BF12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BG12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BH12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BI12" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BJ12" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U13" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AG13" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AM13" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AW13" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J14" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AF14" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AX14" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U15" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="V15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="W15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="X15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Y15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Z15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AA15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AB15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AC15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AD15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AE15" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AY15" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="BW15" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AZ16" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="BA16" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BB16" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BC16" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BD16" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BE16" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BF16" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BG16" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="BY16" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CA17" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AP18" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="CA18" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CB19" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="CI19" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="Q20" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="CB20" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q21" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added water entity type (+...) + int coords -> float coords + different z-index for different entity types + velocity multiplier regions (water is one of them) + springs mostly fixed + entitycreator finds classes by name
Too much for one commit, but most of these changes were pretty much
required to get water working the way I wanted it to work...
</commit_message>
<xml_diff>
--- a/Unnamed Platformer Plan.xlsx
+++ b/Unnamed Platformer Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="23265" windowHeight="10875"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="23265" windowHeight="7335"/>
   </bookViews>
   <sheets>
     <sheet name="Todo" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Brainstorming!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$19</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <oleSize ref="A1:L33"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="102">
   <si>
     <t>1. Implement level serialization</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>Graphics</t>
-  </si>
-  <si>
-    <t>Implement a separate collisionbox that autocrops on load</t>
   </si>
   <si>
     <t>Implement choosing the shape of the collision polygon (circle/square)</t>
@@ -738,8 +735,8 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +766,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -780,7 +777,7 @@
         <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -788,10 +785,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -799,10 +796,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -810,10 +807,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -821,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -832,10 +829,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -843,10 +840,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -854,10 +851,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -865,10 +862,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -876,10 +873,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -887,10 +884,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -905,25 +902,25 @@
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>3</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>40</v>
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="5">
         <v>2</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>78</v>
+      <c r="C16" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -933,8 +930,8 @@
       <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>48</v>
+      <c r="C17" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -944,8 +941,8 @@
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>37</v>
+      <c r="C18" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -953,21 +950,21 @@
         <v>2</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>24</v>
+      <c r="B20" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -975,7 +972,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>92</v>
@@ -986,7 +983,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>93</v>
@@ -997,7 +994,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>94</v>
@@ -1008,7 +1005,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>95</v>
@@ -1019,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>96</v>
@@ -1030,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>97</v>
@@ -1041,51 +1038,51 @@
         <v>2</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="5">
         <v>2</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>2</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>2</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>45</v>
@@ -1096,10 +1093,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1107,10 +1104,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1121,7 +1118,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1129,43 +1126,43 @@
         <v>1</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+      <c r="A37" s="2">
         <v>0</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>23</v>
+      <c r="B37" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="5">
         <v>0</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>80</v>
+      <c r="B38" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1173,22 +1170,14 @@
         <v>0</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>0</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="B40" s="9"/>
     </row>
     <row r="41" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="9"/>
@@ -1218,7 +1207,7 @@
       <c r="B49" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C20">
+  <autoFilter ref="A1:C19">
     <sortState ref="A2:C40">
       <sortCondition descending="1" ref="A1:A20"/>
     </sortState>
@@ -1260,10 +1249,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>20</v>
@@ -1274,10 +1263,10 @@
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1342,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1491,449 +1480,449 @@
   <sheetData>
     <row r="1" spans="1:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK1" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BG2" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BK2" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BX3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BY3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BZ3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CA3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CB3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CC3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CD3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CE3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BW4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BV5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BK6" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BU6" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BK7" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BT7" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BZ7" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BJ8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BK8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BL8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BM8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BN8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BO8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BP8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BQ8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BR8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BS8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BT8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BU8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BV8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BW8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BX8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BY8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BZ8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CA8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CB8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CC8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CD8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CE8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CF8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CG8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="S9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="BJ9" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="BJ9" s="6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q10" s="6" t="s">
+      <c r="T10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="AO10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="BJ10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AO10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BJ10" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="BZ10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="U11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="U11" s="6" t="s">
+      <c r="BJ11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="BJ11" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="BN11" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="U12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AT12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AX12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AY12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BA12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BB12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BE12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BF12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BG12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BH12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BI12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BJ12" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AS12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AT12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AU12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AV12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AW12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AX12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AY12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AZ12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BA12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BB12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BC12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BE12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BF12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BG12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BH12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BI12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="BJ12" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U13" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AG13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW13" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="AM13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AW13" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U14" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AF14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX14" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="AX14" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:88" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="X15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE15" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="W15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="X15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE15" s="6" t="s">
+      <c r="AY15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AY15" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="BW15" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AZ16" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="BA16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BB16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BC16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BD16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BE16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BF16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BG16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BY16" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CA17" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AP18" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="CA18" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="CB19" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="CI19" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="Q20" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="CB20" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Q21" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="13:94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed closed stream bug
</commit_message>
<xml_diff>
--- a/Unnamed Platformer Plan.xlsx
+++ b/Unnamed Platformer Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="23265" windowHeight="7335"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="24060" windowHeight="7335"/>
   </bookViews>
   <sheets>
     <sheet name="Todo" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Brainstorming!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$18</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <oleSize ref="A1:L33"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="103">
   <si>
     <t>1. Implement level serialization</t>
   </si>
@@ -276,9 +276,6 @@
     <t>object type</t>
   </si>
   <si>
-    <t>water (physics slowdown; air timer)</t>
-  </si>
-  <si>
     <t>up&lt;-&gt;down crusher</t>
   </si>
   <si>
@@ -337,6 +334,12 @@
   </si>
   <si>
     <t>Implement image mask -&gt; polygon (1 - create polygon from coordinates of edge pixels; 2 - remove points from polygon and see how much area is reduced; 3 - if area is reduced &lt; x%, allow point removal</t>
+  </si>
+  <si>
+    <t>Bugfix</t>
+  </si>
+  <si>
+    <t>Cannot reload levels after exiting them with F2 (stream issue)</t>
   </si>
 </sst>
 </file>
@@ -735,8 +738,8 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,29 +769,29 @@
         <v>35</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>3</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>43</v>
+      <c r="A3" s="5">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -796,10 +799,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -810,7 +813,7 @@
         <v>80</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -821,7 +824,7 @@
         <v>80</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -832,7 +835,7 @@
         <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -843,7 +846,7 @@
         <v>80</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -854,7 +857,7 @@
         <v>80</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -865,7 +868,7 @@
         <v>80</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -876,7 +879,7 @@
         <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -887,40 +890,40 @@
         <v>80</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="2">
         <v>3</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>3</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>2</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>2</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -930,8 +933,8 @@
       <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>37</v>
+      <c r="C17" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -941,8 +944,8 @@
       <c r="B18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>36</v>
+      <c r="C18" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -950,10 +953,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -964,7 +967,7 @@
         <v>80</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -975,7 +978,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -986,7 +989,7 @@
         <v>80</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -997,7 +1000,7 @@
         <v>80</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1008,7 +1011,7 @@
         <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1019,7 +1022,7 @@
         <v>80</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1030,18 +1033,18 @@
         <v>80</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>2</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>78</v>
+      <c r="B27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1049,32 +1052,32 @@
         <v>2</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>2</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>2</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>44</v>
+      <c r="A30" s="2">
+        <v>1</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1148,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>79</v>
@@ -1207,9 +1210,9 @@
       <c r="B49" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C19">
-    <sortState ref="A2:C40">
-      <sortCondition descending="1" ref="A1:A20"/>
+  <autoFilter ref="A1:C18">
+    <sortState ref="A2:C39">
+      <sortCondition descending="1" ref="A1:A18"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>

<commit_message>
Replaced EntityType enum with dynamic class listing retrieval.
</commit_message>
<xml_diff>
--- a/Unnamed Platformer Plan.xlsx
+++ b/Unnamed Platformer Plan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="24060" windowHeight="7335"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="6195"/>
   </bookViews>
   <sheets>
     <sheet name="Todo" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Brainstorming!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todo!$A$1:$C$17</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <oleSize ref="A1:L33"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="102">
   <si>
     <t>1. Implement level serialization</t>
   </si>
@@ -264,9 +264,6 @@
     <t>Other types:</t>
   </si>
   <si>
-    <t>Improve variety of procedurally generated levels</t>
-  </si>
-  <si>
     <t>object tile chains/grids</t>
   </si>
   <si>
@@ -339,7 +336,7 @@
     <t>Bugfix</t>
   </si>
   <si>
-    <t>Cannot reload levels after exiting them with F2 (stream issue)</t>
+    <t>Create random x-by-y block generator interface</t>
   </si>
 </sst>
 </file>
@@ -739,7 +736,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +766,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -777,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>24</v>
@@ -788,10 +785,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -810,10 +807,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -821,10 +818,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -832,10 +829,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -843,10 +840,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -854,10 +851,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -865,10 +862,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -876,10 +873,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -887,10 +884,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -898,32 +895,32 @@
         <v>3</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="5">
         <v>2</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>77</v>
+      <c r="C16" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -934,29 +931,29 @@
         <v>33</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>37</v>
+      <c r="B18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="2">
         <v>2</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>36</v>
+      <c r="B19" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -964,10 +961,10 @@
         <v>2</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -975,10 +972,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -986,10 +983,10 @@
         <v>2</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -997,10 +994,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1008,32 +1005,32 @@
         <v>2</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="5">
         <v>2</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>95</v>
+      <c r="B25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="5">
         <v>2</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>96</v>
+      <c r="B26" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1041,43 +1038,43 @@
         <v>2</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>2</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>44</v>
+      <c r="A29" s="2">
+        <v>1</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="5">
         <v>1</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>78</v>
+      <c r="B30" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1085,10 +1082,10 @@
         <v>1</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1096,10 +1093,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1110,7 +1107,7 @@
         <v>27</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1118,43 +1115,43 @@
         <v>1</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
+      <c r="A36" s="2">
         <v>0</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>23</v>
+      <c r="B36" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="5">
         <v>0</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>79</v>
+      <c r="B37" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1162,22 +1159,14 @@
         <v>0</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>0</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="B39" s="9"/>
     </row>
     <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
@@ -1210,9 +1199,9 @@
       <c r="B49" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C18">
-    <sortState ref="A2:C39">
-      <sortCondition descending="1" ref="A1:A18"/>
+  <autoFilter ref="A1:C17">
+    <sortState ref="A2:C38">
+      <sortCondition descending="1" ref="A1:A17"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>

<commit_message>
Started converting to Swing-based GUI
</commit_message>
<xml_diff>
--- a/Unnamed Platformer Plan.xlsx
+++ b/Unnamed Platformer Plan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="6195"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="21855" windowHeight="10875"/>
   </bookViews>
   <sheets>
     <sheet name="Todo" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="106">
   <si>
     <t>1. Implement level serialization</t>
   </si>
@@ -337,6 +337,18 @@
   </si>
   <si>
     <t>Create random x-by-y block generator interface</t>
+  </si>
+  <si>
+    <t>Fix bug in grid transparency</t>
+  </si>
+  <si>
+    <t>Fix bug in player graphic corruption when no other graphics on screen</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Setup Jframe to resize along with LWJGL display</t>
   </si>
 </sst>
 </file>
@@ -735,8 +747,8 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1034,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>2</v>
       </c>
@@ -1033,7 +1045,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>2</v>
       </c>
@@ -1045,25 +1057,25 @@
       </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>1</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>31</v>
+      <c r="A28" s="2">
+        <v>2</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1071,21 +1083,21 @@
         <v>1</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="2">
         <v>1</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>38</v>
+      <c r="B31" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1093,10 +1105,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1104,10 +1116,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1115,32 +1127,32 @@
         <v>1</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>0</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>78</v>
+      <c r="A36" s="5">
+        <v>1</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1148,31 +1160,52 @@
         <v>0</v>
       </c>
       <c r="B37" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>0</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>0</v>
+      </c>
+      <c r="B39" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+    <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
         <v>0</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B40" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
-    </row>
-    <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
-    </row>
     <row r="41" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="9"/>
+      <c r="B41" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>
@@ -1200,7 +1233,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C17">
-    <sortState ref="A2:C38">
+    <sortState ref="A2:C40">
       <sortCondition descending="1" ref="A1:A17"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Added ClassLookup to replace some of EntityRef and upcoming Screen class lookups (required global package)
</commit_message>
<xml_diff>
--- a/Unnamed Platformer Plan.xlsx
+++ b/Unnamed Platformer Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="21855" windowHeight="10875"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="23265" windowHeight="10875"/>
   </bookViews>
   <sheets>
     <sheet name="Todo" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="105">
   <si>
     <t>1. Implement level serialization</t>
   </si>
@@ -340,9 +340,6 @@
   </si>
   <si>
     <t>Fix bug in grid transparency</t>
-  </si>
-  <si>
-    <t>Fix bug in player graphic corruption when no other graphics on screen</t>
   </si>
   <si>
     <t>Display</t>
@@ -747,8 +744,8 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,43 +1058,43 @@
         <v>2</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>2</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>103</v>
+      <c r="A29" s="5">
+        <v>1</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="2">
         <v>1</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>31</v>
+      <c r="B30" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="5">
         <v>1</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>77</v>
+      <c r="B31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1105,10 +1102,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1116,10 +1113,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1130,7 +1127,7 @@
         <v>27</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1138,43 +1135,43 @@
         <v>1</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+      <c r="A37" s="2">
         <v>0</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>23</v>
+      <c r="B37" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="5">
         <v>0</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>78</v>
+      <c r="B38" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1182,30 +1179,22 @@
         <v>0</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>0</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>30</v>
+      <c r="B40" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="9"/>

</xml_diff>